<commit_message>
changed game play data
</commit_message>
<xml_diff>
--- a/data/config/actor.xlsx
+++ b/data/config/actor.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="13365" windowHeight="4395"/>
+    <workbookView xWindow="396" yWindow="108" windowWidth="13368" windowHeight="4392"/>
   </bookViews>
   <sheets>
     <sheet name="actor" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -32,18 +28,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>atk_dis</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>at_dis</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk_speed</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>icon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -52,99 +36,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>skill_loop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>list</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>speed</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>radius</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_energy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damaged_get</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damaged_put</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>die_put</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>head_wolf</t>
-  </si>
-  <si>
     <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pos</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>paladin01</t>
-  </si>
-  <si>
-    <t>wolf01</t>
-  </si>
-  <si>
-    <t>mage01</t>
-  </si>
-  <si>
-    <t>banshee01</t>
-  </si>
-  <si>
-    <t>head_banshee</t>
-  </si>
-  <si>
-    <t>head_mage</t>
-  </si>
-  <si>
-    <t>head_paladin</t>
-  </si>
-  <si>
-    <t>1,1,1,2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2,0,1,1,2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,1,2,0,1,1,1,2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,1,1,2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,7 +691,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -865,7 +765,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -900,7 +799,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1076,288 +974,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.375" customWidth="1"/>
-    <col min="8" max="9" width="8.125" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
-    <col min="11" max="12" width="14.75" customWidth="1"/>
-    <col min="13" max="13" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="9" width="8.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="11" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>0.5</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>0.7</v>
-      </c>
-      <c r="I3">
-        <v>2.5</v>
-      </c>
-      <c r="J3">
-        <v>500</v>
-      </c>
-      <c r="K3">
-        <v>1000</v>
-      </c>
-      <c r="L3">
-        <v>300</v>
-      </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>5.6</v>
-      </c>
-      <c r="F4">
-        <v>2.8</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>2.5</v>
-      </c>
-      <c r="J4">
-        <v>500</v>
-      </c>
-      <c r="K4">
-        <v>1000</v>
-      </c>
-      <c r="L4">
-        <v>300</v>
-      </c>
-      <c r="M4">
-        <v>1000</v>
-      </c>
-      <c r="N4" t="s">
-        <v>30</v>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5">
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>2.8</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-      <c r="I5">
-        <v>2.5</v>
-      </c>
-      <c r="J5">
-        <v>500</v>
-      </c>
-      <c r="K5">
-        <v>1000</v>
-      </c>
-      <c r="L5">
-        <v>300</v>
-      </c>
-      <c r="M5">
-        <v>1000</v>
-      </c>
-      <c r="N5" t="s">
-        <v>31</v>
+      <c r="C5">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.5</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.7</v>
-      </c>
-      <c r="I6">
-        <v>2.5</v>
-      </c>
-      <c r="J6">
-        <v>500</v>
-      </c>
-      <c r="K6">
-        <v>1000</v>
-      </c>
-      <c r="L6">
-        <v>300</v>
-      </c>
-      <c r="M6">
-        <v>1000</v>
-      </c>
-      <c r="N6" t="s">
-        <v>32</v>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>